<commit_message>
Added login and register views, viewmodels, and styles to WPF
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e242afc395d22f1/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{CDECF54E-3161-4D8D-AA92-1EE1699C540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A013BB9B-121B-4A71-AC25-B0EDD4274281}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D2C518-1994-4489-B767-5D260B2E5DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
   <si>
     <t>Database</t>
   </si>
@@ -99,10 +99,6 @@
   </si>
   <si>
     <t>As a user of the system, I need to be able to register myself with a username and password.</t>
-  </si>
-  <si>
-    <t>1. A new registered user starts with an initial balance of 1,000 TE Bucks.
-2. The ability to register has been provided in your starter code.</t>
   </si>
   <si>
     <t>As a user of the system, I need to be able to log in using my registered username and password.</t>
@@ -521,6 +517,15 @@
       <t>4. Move conn string into config</t>
     </r>
   </si>
+  <si>
+    <t>1. A new registered user starts with an initial balance of 1,000 Funny Bucks.</t>
+  </si>
+  <si>
+    <t>d7b837d</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/22114260/how-to-use-styles-defined-in-resourcedictionary</t>
+  </si>
 </sst>
 </file>
 
@@ -581,7 +586,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,6 +602,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -663,6 +674,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -729,10 +746,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1045,7 +1058,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B2" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1158,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1157,10 +1170,10 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -1180,19 +1193,19 @@
         <v>0</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="71.25" x14ac:dyDescent="0.45">
@@ -1200,44 +1213,48 @@
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B5" s="16">
+        <v>2</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="E5" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="2:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="4">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1248,7 +1265,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1260,10 +1277,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1274,7 +1291,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1286,7 +1303,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1298,10 +1315,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1312,7 +1329,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1324,10 +1341,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1354,7 +1371,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1377,7 +1394,7 @@
   <sheetData>
     <row r="5" spans="3:20" ht="409.5" x14ac:dyDescent="0.45">
       <c r="T5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.45">
@@ -1385,42 +1402,42 @@
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C8" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C9" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C12" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C14" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C15" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C17" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1445,16 +1462,16 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.45">
@@ -1465,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.45">
@@ -1479,10 +1496,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.45">
@@ -1493,10 +1510,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
@@ -1507,10 +1524,10 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:5" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
@@ -1521,10 +1538,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.45">
@@ -1535,10 +1552,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.45">
@@ -1549,10 +1566,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1578,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -1586,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Added register user functionality to WPF
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D2C518-1994-4489-B767-5D260B2E5DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B1F8DA-A38B-46C4-9C7C-507730B22C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
   <sheets>
     <sheet name="00 Project Description" sheetId="3" r:id="rId1"/>
@@ -443,10 +443,6 @@
     <t>(Allowing multiple accounts per user could be a new feature down the road; I added this to 99 TODO)</t>
   </si>
   <si>
-    <t>2f8f108
-cc9147f</t>
-  </si>
-  <si>
     <r>
       <t>1. Create DAL project</t>
     </r>
@@ -521,10 +517,18 @@
     <t>1. A new registered user starts with an initial balance of 1,000 Funny Bucks.</t>
   </si>
   <si>
-    <t>d7b837d</t>
-  </si>
-  <si>
     <t>https://stackoverflow.com/questions/22114260/how-to-use-styles-defined-in-resourcedictionary</t>
+  </si>
+  <si>
+    <t>d7b837d
+ae3323b</t>
+  </si>
+  <si>
+    <t>cc9147f
+2f8f108
+ead8453
+cf62796
+ce6f408</t>
   </si>
 </sst>
 </file>
@@ -612,7 +616,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -635,11 +639,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF002060"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF002060"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF002060"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF002060"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF002060"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -680,6 +710,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1156,9 +1192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93111F4B-B752-4F62-AA87-F788E68BCD52}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1216,7 +1252,7 @@
         <v>58</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>61</v>
@@ -1225,7 +1261,7 @@
         <v>49</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -1236,29 +1272,29 @@
         <v>18</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>68</v>
-      </c>
       <c r="F5" s="17"/>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="18" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="4">
+      <c r="B6" s="16">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
@@ -1351,6 +1387,9 @@
       <c r="G13" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G5:G6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Debugged register user in WPF; code cleanup on entire solution
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B1F8DA-A38B-46C4-9C7C-507730B22C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFDFD97-9EAC-40DB-BC68-79150D7C57F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
   <si>
     <t>Database</t>
   </si>
@@ -410,10 +410,6 @@
     <t>First and last names for users</t>
   </si>
   <si>
-    <t>https://learn.microsoft.com/en-us/ef/core/managing-schemas/scaffolding/?tabs=dotnet-core-cli
-My customizations are in FunnyMoneyTransferContext.cs::OnModelCreatingPartial()</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">And I enforced a relationship in my db differently than indicated here; </t>
     </r>
@@ -517,18 +513,19 @@
     <t>1. A new registered user starts with an initial balance of 1,000 Funny Bucks.</t>
   </si>
   <si>
-    <t>https://stackoverflow.com/questions/22114260/how-to-use-styles-defined-in-resourcedictionary</t>
-  </si>
-  <si>
-    <t>d7b837d
-ae3323b</t>
-  </si>
-  <si>
     <t>cc9147f
 2f8f108
 ead8453
 cf62796
 ce6f408</t>
+  </si>
+  <si>
+    <t>d7b837d
+ae3323b
+fbda41c8</t>
+  </si>
+  <si>
+    <t>My customizations are in FunnyMoneyTransferContext.cs::OnModelCreatingPartial()</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1191,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1252,16 +1249,16 @@
         <v>58</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>49</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -1272,14 +1269,12 @@
         <v>18</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>66</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1466,12 +1461,12 @@
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C14" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C15" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Added current balance class to data project
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFDFD97-9EAC-40DB-BC68-79150D7C57F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BEF867-EDE3-45BC-98FB-C2E08547715B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
   <sheets>
     <sheet name="00 Project Description" sheetId="3" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="05 Business Rules" sheetId="6" r:id="rId6"/>
     <sheet name="99 TODO" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'05 Business Rules'!$B$2:$F$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="94">
   <si>
     <t>Database</t>
   </si>
@@ -66,9 +69,6 @@
   </si>
   <si>
     <t>RestSharp</t>
-  </si>
-  <si>
-    <t>WPF? Web?</t>
   </si>
   <si>
     <t>Layer</t>
@@ -301,22 +301,10 @@
     <t>Transfer type descriptions must be unique in the transfer_types table</t>
   </si>
   <si>
-    <t>unique constraint on this column</t>
-  </si>
-  <si>
     <t>Transfer status descriptions must be unique in the transfer_statuses table</t>
   </si>
   <si>
     <t>Usernames must be unique in the users table</t>
-  </si>
-  <si>
-    <t>transfers must have different 'from' and 'to' accounts</t>
-  </si>
-  <si>
-    <t>transfer amounts must be greater than zero</t>
-  </si>
-  <si>
-    <t>check constraint in transfers table</t>
   </si>
   <si>
     <t>Create database</t>
@@ -520,19 +508,116 @@
 ce6f408</t>
   </si>
   <si>
+    <t>My customizations are in FunnyMoneyTransferContext.cs::OnModelCreatingPartial()</t>
+  </si>
+  <si>
+    <t>A lot of code/xaml is duplicated between the register user and login user xaml and viewmodels - refactor out the repeated code</t>
+  </si>
+  <si>
+    <t>WPF; others later?</t>
+  </si>
+  <si>
+    <t>I am not using the starter code (JWT) and thus logging in does not return a token
+Instead I am keeping track of the LoggedInUser in the login viewmodel; hopefully this can be passed up maybe even to application so it can be used throughout the application</t>
+  </si>
+  <si>
+    <t>DataAccess</t>
+  </si>
+  <si>
+    <t>Username is required on the user entity</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Transfer Types</t>
+  </si>
+  <si>
+    <t>Transfer Statuses</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
+    <t>Starting Balances</t>
+  </si>
+  <si>
+    <t>Transfers</t>
+  </si>
+  <si>
+    <t>Password max length = 50</t>
+  </si>
+  <si>
+    <t>WPF</t>
+  </si>
+  <si>
+    <t>Username not null, empty, or whitespace</t>
+  </si>
+  <si>
+    <t>Viewmodel validate() method in register user and login user</t>
+  </si>
+  <si>
+    <t>Username max length = 50</t>
+  </si>
+  <si>
+    <t>Username must be unique</t>
+  </si>
+  <si>
+    <t>Unique constraint on this column</t>
+  </si>
+  <si>
+    <t>Unique constraint on this entity</t>
+  </si>
+  <si>
+    <t>User ids must be unique in the accounts entity, i.e. one user, one account and vice versa</t>
+  </si>
+  <si>
+    <t>Account ids must be unique in the starting balances entity, i.e., one account, one starting balance and vice versa</t>
+  </si>
+  <si>
+    <t>Transfers must have different 'from' and 'to' accounts</t>
+  </si>
+  <si>
+    <t>Transfer amounts must be greater than zero</t>
+  </si>
+  <si>
+    <t>Check constraint in transfers table</t>
+  </si>
+  <si>
+    <t>Check constraint on this entity</t>
+  </si>
+  <si>
+    <t>Set in the xaml for register user and login user</t>
+  </si>
+  <si>
+    <t>Viewmodel validate() method in register user</t>
+  </si>
+  <si>
+    <t>Usernames must be unique in the users entity</t>
+  </si>
+  <si>
+    <t>Set on entity model</t>
+  </si>
+  <si>
+    <t>I am leaving out the API and thus the client services; since this is my first project with EF I don't want to introduce the complexities of disconnected entities (server side vs. client side)</t>
+  </si>
+  <si>
     <t>d7b837d
 ae3323b
-fbda41c8</t>
-  </si>
-  <si>
-    <t>My customizations are in FunnyMoneyTransferContext.cs::OnModelCreatingPartial()</t>
+fbda41c
+7475fee
+f46696a
+1fc92f6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,14 +636,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -586,8 +663,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,14 +700,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -662,6 +750,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF002060"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -669,50 +766,46 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1091,7 +1184,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1101,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBB70B6-EAED-4421-B195-4B7AC27E04D2}">
-  <dimension ref="B2:D7"/>
+  <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1114,70 +1207,73 @@
     <col min="4" max="4" width="26.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1189,9 +1285,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93111F4B-B752-4F62-AA87-F788E68BCD52}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1203,92 +1299,98 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="B3" s="12">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B5" s="12">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="57" x14ac:dyDescent="0.45">
-      <c r="B3" s="13">
-        <v>0</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B5" s="16">
-        <v>2</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B6" s="12">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="16">
-        <v>3</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="F6" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="G6" s="19"/>
     </row>
     <row r="7" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -1296,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1308,10 +1410,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1322,7 +1424,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1334,7 +1436,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1346,10 +1448,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1360,7 +1462,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1372,10 +1474,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1395,7 +1497,7 @@
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1405,7 +1507,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1428,50 +1530,50 @@
   <sheetData>
     <row r="5" spans="3:20" ht="409.5" x14ac:dyDescent="0.45">
       <c r="T5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.45">
-      <c r="C6" s="12"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C7" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C10" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C12" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C14" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C15" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C17" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1482,131 +1584,329 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1174A8-C05F-4D78-B681-DE0740FA8BD6}">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="59.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.1328125" customWidth="1"/>
+    <col min="5" max="5" width="59.265625" customWidth="1"/>
+    <col min="6" max="6" width="29.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B3" s="2">
+    </row>
+    <row r="3" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="17">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B4" s="2">
+      <c r="D3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B5" s="2">
+        <v>65</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B5" s="17">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B6" s="2">
+      <c r="D5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B6" s="17">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B7" s="2">
+        <v>65</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B7" s="17">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B8" s="2">
+      <c r="D7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B8" s="17">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B9" s="2">
+      <c r="D8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B9" s="17">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>46</v>
+      <c r="D9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B10" s="17">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B11" s="17">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B12" s="17">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B13" s="17">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B14" s="17">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B15" s="17">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="17">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="17">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="17">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B19" s="17">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F19">
+    <sortCondition ref="D3:D19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1624,12 +1924,12 @@
     <col min="3" max="3" width="45.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>55</v>
+      <c r="C2" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -1637,12 +1937,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="2"/>

</xml_diff>

<commit_message>
Added balance view, viewmodel, and styles to WPF
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BEF867-EDE3-45BC-98FB-C2E08547715B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7640F71F-79EF-488A-99E4-E08A25AB31AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
   <sheets>
     <sheet name="00 Project Description" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="95">
   <si>
     <t>Database</t>
   </si>
@@ -612,6 +612,9 @@
 f46696a
 1fc92f6</t>
   </si>
+  <si>
+    <t>a916c29</t>
+  </si>
 </sst>
 </file>
 
@@ -681,7 +684,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,6 +700,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -763,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -806,6 +815,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1286,8 +1301,8 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1394,16 +1409,18 @@
       <c r="G6" s="19"/>
     </row>
     <row r="7" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B7" s="4">
+      <c r="B7" s="20">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="8" spans="2:7" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B8" s="4">

</xml_diff>

<commit_message>
Added customizations to regenerated data context
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7640F71F-79EF-488A-99E4-E08A25AB31AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DC209B-EC85-45A8-A17A-7323204A3F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="5" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
   <sheets>
     <sheet name="00 Project Description" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="99 TODO" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'05 Business Rules'!$B$2:$F$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'05 Business Rules'!$B$2:$F$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
   <si>
     <t>Database</t>
   </si>
@@ -613,7 +613,18 @@
 1fc92f6</t>
   </si>
   <si>
-    <t>a916c29</t>
+    <t>a916c29
+407be7b
+0226640</t>
+  </si>
+  <si>
+    <t>Enums for TransferType and TransferStatus https://itnext.io/how-to-use-enums-when-using-entity-framework-core-with-c-bb634692a4b0</t>
+  </si>
+  <si>
+    <t>Transfer status descriptions must be unique in the transfer_statuses entity</t>
+  </si>
+  <si>
+    <t>Transfer type descriptions must be unique in the transfer_types entity</t>
   </si>
 </sst>
 </file>
@@ -1300,9 +1311,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93111F4B-B752-4F62-AA87-F788E68BCD52}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1408,33 +1419,33 @@
       </c>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B7" s="20">
+    <row r="7" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B7" s="12">
         <v>4</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="B8" s="4">
+      <c r="B8" s="20">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B9" s="5">
@@ -1601,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1174A8-C05F-4D78-B681-DE0740FA8BD6}">
-  <dimension ref="B2:F19"/>
+  <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1635,101 +1646,101 @@
       <c r="B3" s="17">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>80</v>
+      <c r="E3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="17">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>81</v>
+      <c r="E4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B5" s="17">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>80</v>
+      <c r="E5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B6" s="17">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>81</v>
+      <c r="E6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B7" s="17">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>80</v>
+      <c r="E7" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="17">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="D8" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1737,50 +1748,50 @@
       <c r="B9" s="17">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>86</v>
+      <c r="C9" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" s="17">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>86</v>
+      <c r="D10" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11" s="17">
         <v>9</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1788,16 +1799,16 @@
       <c r="B12" s="17">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1805,124 +1816,158 @@
       <c r="B13" s="17">
         <v>11</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>80</v>
+      <c r="D13" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B14" s="17">
         <v>12</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>81</v>
+      <c r="C14" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B15" s="17">
         <v>13</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B16" s="17">
         <v>14</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" s="17">
         <v>15</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>77</v>
+      <c r="E17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B18" s="17">
         <v>16</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>77</v>
+      <c r="E18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B19" s="17">
         <v>17</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B20" s="17">
+        <v>18</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B21" s="17">
+        <v>19</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F21" s="5" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F19">
-    <sortCondition ref="D3:D19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F21">
+    <sortCondition ref="D3:D21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1933,7 +1978,7 @@
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1965,9 +2010,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+    <row r="5" spans="2:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="2"/>

</xml_diff>

<commit_message>
Updates to balance view and viewmodel, and login- and register- user viewmodels
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DC209B-EC85-45A8-A17A-7323204A3F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3FD99B-67A4-446A-B39E-1E256E6CED6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="5" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
   <sheets>
     <sheet name="00 Project Description" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="99">
   <si>
     <t>Database</t>
   </si>
@@ -625,6 +625,9 @@
   </si>
   <si>
     <t>Transfer type descriptions must be unique in the transfer_types entity</t>
+  </si>
+  <si>
+    <t>7ad87a7</t>
   </si>
 </sst>
 </file>
@@ -1311,9 +1314,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93111F4B-B752-4F62-AA87-F788E68BCD52}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1445,7 +1448,9 @@
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
+      <c r="G8" s="21" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="9" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B9" s="5">
@@ -1614,7 +1619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1174A8-C05F-4D78-B681-DE0740FA8BD6}">
   <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fine tuned the main window navigation in WPF
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3FD99B-67A4-446A-B39E-1E256E6CED6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D376F2-C8F1-4DEB-BEFF-693F4ED8662A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
@@ -627,7 +627,10 @@
     <t>Transfer type descriptions must be unique in the transfer_types entity</t>
   </si>
   <si>
-    <t>7ad87a7</t>
+    <t>7ad87a7
+1202b67
+15ab379
+c98d69f</t>
   </si>
 </sst>
 </file>
@@ -1314,9 +1317,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93111F4B-B752-4F62-AA87-F788E68BCD52}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Code clean up on entire solution
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D376F2-C8F1-4DEB-BEFF-693F4ED8662A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED6718F-08C6-4152-92E2-65C1639C4B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
@@ -630,7 +630,12 @@
     <t>7ad87a7
 1202b67
 15ab379
-c98d69f</t>
+c98d69f
+8a2a03f
+b71dd63
+6b22dc8
+499693b
+35726b5</t>
   </si>
 </sst>
 </file>
@@ -828,16 +833,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1318,7 +1323,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1403,7 +1408,7 @@
       <c r="F5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="20" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1423,7 +1428,7 @@
       <c r="F6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B7" s="12">
@@ -1439,19 +1444,19 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="B8" s="20">
+    <row r="8" spans="2:7" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B8" s="18">
         <v>5</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added send transfer view and viewmodel in WPF
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED6718F-08C6-4152-92E2-65C1639C4B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE0BA11-5BCB-44C3-ADB9-8F283D47B8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
@@ -635,7 +635,9 @@
 b71dd63
 6b22dc8
 499693b
-35726b5</t>
+35726b5
+2344cf7
+c46671f</t>
   </si>
 </sst>
 </file>
@@ -1322,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93111F4B-B752-4F62-AA87-F788E68BCD52}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
@@ -1444,7 +1446,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B8" s="18">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Fixed issue with send and request buttons not showing up in users list in WPF
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE0BA11-5BCB-44C3-ADB9-8F283D47B8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BF8D2C-FC48-4884-832B-5F4CE79DDD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
@@ -637,7 +637,10 @@
 499693b
 35726b5
 2344cf7
-c46671f</t>
+c46671f
+0f3d9f2
+f628fc6
+Commit 5de5df1</t>
   </si>
 </sst>
 </file>
@@ -1324,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93111F4B-B752-4F62-AA87-F788E68BCD52}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1446,7 +1449,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" ht="213.75" x14ac:dyDescent="0.45">
       <c r="B8" s="18">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Complete reorganization of MainWindow layout and navigation; now going for a dashboard type view with most components visible at the same time
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BF8D2C-FC48-4884-832B-5F4CE79DDD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04CB754-4ACF-4CA4-89B3-AF491547929A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
@@ -640,7 +640,9 @@
 c46671f
 0f3d9f2
 f628fc6
-Commit 5de5df1</t>
+Commit 5de5df1
+fe4d739
+1a30f5a</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1451,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" ht="242.25" x14ac:dyDescent="0.45">
       <c r="B8" s="18">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Changes to Main Window in WPF to accomodate combining of logged in user view and balance view
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04CB754-4ACF-4CA4-89B3-AF491547929A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B92840-707D-48A5-A852-6F7C12722BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
@@ -642,7 +642,10 @@
 f628fc6
 Commit 5de5df1
 fe4d739
-1a30f5a</t>
+1a30f5a
+7490abd
+aac65a9
+6a070dc</t>
   </si>
 </sst>
 </file>
@@ -1329,9 +1332,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93111F4B-B752-4F62-AA87-F788E68BCD52}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1451,7 +1454,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" ht="285" x14ac:dyDescent="0.45">
       <c r="B8" s="18">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Code cleanup on entire solution
</commit_message>
<xml_diff>
--- a/Documentation/Funny Money Transfer Project Plan.xlsx
+++ b/Documentation/Funny Money Transfer Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\FunnyMoneyTransfer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B92840-707D-48A5-A852-6F7C12722BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89573743-0A80-45D7-929D-074508ADDF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="786" activeTab="2" xr2:uid="{A6246D22-F85E-4B48-AAD5-08599A3CA99F}"/>
   </bookViews>
@@ -640,12 +640,18 @@
 c46671f
 0f3d9f2
 f628fc6
-Commit 5de5df1
+5de5df1
 fe4d739
 1a30f5a
 7490abd
 aac65a9
-6a070dc</t>
+6a070dc
+c81e828
+c70814e
+7b4461a
+cd7a0bd
+1abfbc4
+65f4e1c</t>
   </si>
 </sst>
 </file>
@@ -1333,8 +1339,8 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1454,7 +1460,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="285" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" ht="356.25" x14ac:dyDescent="0.45">
       <c r="B8" s="18">
         <v>5</v>
       </c>

</xml_diff>